<commit_message>
Additions to FinalProject presentation
</commit_message>
<xml_diff>
--- a/FinalProject/Docs/Townes_POLS6310_2019_Spring_FinalProject_Charts_v00.xlsx
+++ b/FinalProject/Docs/Townes_POLS6310_2019_Spring_FinalProject_Charts_v00.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="108">
   <si>
     <t>Obligation (dollars in thousands)</t>
   </si>
@@ -327,6 +327,18 @@
   </si>
   <si>
     <t>SBIR Pct of Potential</t>
+  </si>
+  <si>
+    <t>Set-aside</t>
+  </si>
+  <si>
+    <t>SBIR Potential Pct of Industry Ideal</t>
+  </si>
+  <si>
+    <t>SBIR Potential as Pct of Industry Ideal</t>
+  </si>
+  <si>
+    <t>Actual SBIR Pct of Industry</t>
   </si>
 </sst>
 </file>
@@ -433,8 +445,6 @@
     </xf>
     <xf numFmtId="43" fontId="0" fillId="4" borderId="0" xfId="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
@@ -447,6 +457,8 @@
     <xf numFmtId="10" fontId="0" fillId="4" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -511,11 +523,14 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>SBIR Pct of Industry</c:v>
+                  <c:v>Actual SBIR Pct of Industry</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
           <c:xVal>
             <c:numRef>
               <c:f>Chart!$A$2:$A$27</c:f>
@@ -692,19 +707,212 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chart!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Set-aside</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:dLbls>
+            <c:delete val="1"/>
+          </c:dLbls>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Chart!$A$2:$A$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Chart!$C$2:$C$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.2500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
+          <c:showVal val="1"/>
           <c:showCatName val="0"/>
           <c:showSerName val="0"/>
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="171792640"/>
-        <c:axId val="161184768"/>
+        <c:axId val="159665152"/>
+        <c:axId val="159671040"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="171792640"/>
+        <c:axId val="159665152"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2015"/>
@@ -716,13 +924,13 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161184768"/>
+        <c:crossAx val="159671040"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161184768"/>
+        <c:axId val="159671040"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -733,7 +941,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171792640"/>
+        <c:crossAx val="159665152"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -804,7 +1012,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Chart!$S$1</c:f>
+              <c:f>Chart!$T$1</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -815,7 +1023,7 @@
           </c:tx>
           <c:xVal>
             <c:numRef>
-              <c:f>Chart!$R$2:$R$27</c:f>
+              <c:f>Chart!$S$2:$S$27</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="26"/>
@@ -902,7 +1110,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Chart!$S$2:$S$27</c:f>
+              <c:f>Chart!$T$2:$T$27</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="26"/>
@@ -997,11 +1205,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="178043136"/>
-        <c:axId val="171819776"/>
+        <c:axId val="159699328"/>
+        <c:axId val="159700864"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="178043136"/>
+        <c:axId val="159699328"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2015"/>
@@ -1013,12 +1221,12 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="171819776"/>
+        <c:crossAx val="159700864"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="171819776"/>
+        <c:axId val="159700864"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1029,7 +1237,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="178043136"/>
+        <c:crossAx val="159699328"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1051,20 +1259,764 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Targets for Small</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> Business R&amp;D Funding</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chart!$AM$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Actual SBIR Pct of Industry</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Chart!$AL$2:$AL$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Chart!$AM$2:$AM$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.5687027579162412E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.8284217618070749E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.7092164008498965E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.3096859591647638E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.3564254028087435E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.8593270957563973E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>3.0167446944406033E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>3.5233025560722234E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.5297669273030692E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>3.4372024061413653E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3.9052028113747105E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>4.8837151650157416E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>4.0877259972808007E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>4.4030667534924864E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>4.4765475208358566E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>4.1536939381475367E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>4.0072430526595142E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>3.7588499213079329E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>3.7889508960268097E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>5.1054109277875501E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>5.5241337110587443E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>4.4343699260644381E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>3.7907077296420941E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>4.2656195131108195E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>4.5385307495546069E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>4.4417976133047585E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chart!$AN$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SBIR Potential as Pct of Industry Ideal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent3">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent3">
+                    <a:lumMod val="75000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Chart!$AL$2:$AL$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Chart!$AN$2:$AN$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>4.5346288932896141E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>5.221862614201879E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4.8527854451927276E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>6.5700764877829623E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.1988122820615633E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.2662367756665481E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.4276464979243265E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.9313486905973788E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.5433980174787908E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9.2905487302346657E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.1174960330668553</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.13157754429262633</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.12645530295920784</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.1225168202707379</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.12643900059712318</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.10968641899381416</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>9.8048230088917832E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>8.8303613220131097E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>9.0560523572040891E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.12329445793584255</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.13953621098603594</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>9.2789552446865001E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>8.5652985219278763E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>9.0822554345615064E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>9.9265533835264139E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>8.8456951293445982E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Chart!$AO$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Set-aside</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:ln>
+                <a:solidFill>
+                  <a:schemeClr val="accent2"/>
+                </a:solidFill>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>Chart!$AL$2:$AL$27</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1990</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1991</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1992</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1993</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1994</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1995</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1996</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1997</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2000</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2002</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2003</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2004</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2005</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2006</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2007</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2008</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2009</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2010</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2011</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2012</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2013</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2014</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>Chart!$AO$2:$AO$27</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="26"/>
+                <c:pt idx="0">
+                  <c:v>1.2500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.2500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.2500000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.5000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.5999999999999999E-2</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>2.7E-2</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>2.8000000000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>2.9000000000000001E-2</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="164856192"/>
+        <c:axId val="164854400"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="164856192"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="2015"/>
+          <c:min val="1990"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="out"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="164854400"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="164854400"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="164856192"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+  </c:spPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>142874</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>95249</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>71436</xdr:rowOff>
+      <xdr:rowOff>61911</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>600075</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>552450</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1085,16 +2037,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>85724</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>180974</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>90486</xdr:rowOff>
+      <xdr:rowOff>33336</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>32</xdr:col>
-      <xdr:colOff>552450</xdr:colOff>
+      <xdr:col>34</xdr:col>
+      <xdr:colOff>38100</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1108,6 +2060,36 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>41</xdr:col>
+      <xdr:colOff>228599</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>71436</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>53</xdr:col>
+      <xdr:colOff>523875</xdr:colOff>
+      <xdr:row>26</xdr:row>
+      <xdr:rowOff>114299</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1403,10 +2385,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I28"/>
+  <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J1" sqref="J1"/>
+      <selection activeCell="J2" sqref="J2:J28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1419,47 +2401,51 @@
     <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="32.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+    <row r="1" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="17" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="14"/>
-      <c r="C1" s="14"/>
-      <c r="D1" s="14"/>
-      <c r="E1" s="14"/>
-    </row>
-    <row r="2" spans="1:9" s="4" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="15" t="s">
+      <c r="B1" s="18"/>
+      <c r="C1" s="18"/>
+      <c r="D1" s="18"/>
+      <c r="E1" s="18"/>
+    </row>
+    <row r="2" spans="1:10" s="4" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="13" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="15" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="13" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="D2" s="13" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="E2" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="13" t="s">
         <v>100</v>
       </c>
-      <c r="G2" s="15" t="s">
+      <c r="G2" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="H2" s="15" t="s">
+      <c r="H2" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="I2" s="15" t="s">
+      <c r="I2" s="13" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2" s="13" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1990</v>
       </c>
@@ -1483,15 +2469,19 @@
         <v>1.5687027579162412E-2</v>
       </c>
       <c r="H3" s="1">
-        <f>(D3/0.15)+(E3/0.5)</f>
+        <f>($D3/0.15)+($E3/0.5)</f>
         <v>1472382</v>
       </c>
       <c r="I3" s="2">
         <f>B3/H3</f>
         <v>0.31291336079903176</v>
       </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J3" s="2">
+        <f>(($D3/0.15)+($E3/0.5))/(($D3/0.15)+($E3/0.5)+(($F3-(($D3/0.15)+($E3/0.5)))/0.9))</f>
+        <v>4.5346288932896141E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1991</v>
       </c>
@@ -1522,8 +2512,12 @@
         <f t="shared" ref="I4:I28" si="2">B4/H4</f>
         <v>0.31696110663001692</v>
       </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J4" s="2">
+        <f t="shared" ref="J4:J28" si="3">(($D4/0.15)+($E4/0.5))/(($D4/0.15)+($E4/0.5)+(($F4-(($D4/0.15)+($E4/0.5)))/0.9))</f>
+        <v>5.221862614201879E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1992</v>
       </c>
@@ -1554,8 +2548,12 @@
         <f t="shared" si="2"/>
         <v>0.31870133940698325</v>
       </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J5" s="2">
+        <f t="shared" si="3"/>
+        <v>4.8527854451927276E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="8">
         <v>1993</v>
       </c>
@@ -1586,8 +2584,12 @@
         <f t="shared" si="2"/>
         <v>0.31870133940698325</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J6" s="12">
+        <f t="shared" si="3"/>
+        <v>6.5700764877829623E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1994</v>
       </c>
@@ -1618,8 +2620,12 @@
         <f t="shared" si="2"/>
         <v>0.29695819850537519</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7" s="2">
+        <f t="shared" si="3"/>
+        <v>7.1988122820615633E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1995</v>
       </c>
@@ -1650,8 +2656,12 @@
         <f t="shared" si="2"/>
         <v>0.31417322434052192</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J8" s="2">
+        <f t="shared" si="3"/>
+        <v>8.2662367756665481E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1996</v>
       </c>
@@ -1682,8 +2692,12 @@
         <f t="shared" si="2"/>
         <v>0.32517907384116584</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J9" s="2">
+        <f t="shared" si="3"/>
+        <v>8.4276464979243265E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1997</v>
       </c>
@@ -1714,8 +2728,12 @@
         <f t="shared" si="2"/>
         <v>0.32281249471455076</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J10" s="2">
+        <f t="shared" si="3"/>
+        <v>9.9313486905973788E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1998</v>
       </c>
@@ -1746,8 +2764,12 @@
         <f t="shared" si="2"/>
         <v>0.33640808016064533</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J11" s="2">
+        <f t="shared" si="3"/>
+        <v>9.5433980174787908E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="8">
         <v>1999</v>
       </c>
@@ -1778,8 +2800,12 @@
         <f t="shared" si="2"/>
         <v>0.33640808016064533</v>
       </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J12" s="12">
+        <f t="shared" si="3"/>
+        <v>9.2905487302346657E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2000</v>
       </c>
@@ -1810,8 +2836,12 @@
         <f t="shared" si="2"/>
         <v>0.30303721931421135</v>
       </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J13" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1174960330668553</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2001</v>
       </c>
@@ -1842,8 +2872,12 @@
         <f t="shared" si="2"/>
         <v>0.33893339454943977</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14" s="2">
+        <f t="shared" si="3"/>
+        <v>0.13157754429262633</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2002</v>
       </c>
@@ -1874,8 +2908,12 @@
         <f t="shared" si="2"/>
         <v>0.29501687736228793</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12645530295920784</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2003</v>
       </c>
@@ -1906,8 +2944,12 @@
         <f t="shared" si="2"/>
         <v>0.32784927351810844</v>
       </c>
-    </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J16" s="2">
+        <f t="shared" si="3"/>
+        <v>0.1225168202707379</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2004</v>
       </c>
@@ -1938,8 +2980,12 @@
         <f t="shared" si="2"/>
         <v>0.32311974698661361</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12643900059712318</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2005</v>
       </c>
@@ -1970,8 +3016,12 @@
         <f t="shared" si="2"/>
         <v>0.34497296569717978</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18" s="2">
+        <f t="shared" si="3"/>
+        <v>0.10968641899381416</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2006</v>
       </c>
@@ -2002,8 +3052,12 @@
         <f t="shared" si="2"/>
         <v>0.37183833435567315</v>
       </c>
-    </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J19" s="2">
+        <f t="shared" si="3"/>
+        <v>9.8048230088917832E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>2007</v>
       </c>
@@ -2034,8 +3088,12 @@
         <f t="shared" si="2"/>
         <v>0.38686490932385847</v>
       </c>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J20" s="2">
+        <f t="shared" si="3"/>
+        <v>8.8303613220131097E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>2008</v>
       </c>
@@ -2066,8 +3124,12 @@
         <f t="shared" si="2"/>
         <v>0.38033887264106064</v>
       </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J21" s="2">
+        <f t="shared" si="3"/>
+        <v>9.0560523572040891E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>2009</v>
       </c>
@@ -2098,8 +3160,12 @@
         <f t="shared" si="2"/>
         <v>0.3777798937824654</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22" s="2">
+        <f t="shared" si="3"/>
+        <v>0.12329445793584255</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>2010</v>
       </c>
@@ -2130,8 +3196,12 @@
         <f t="shared" si="2"/>
         <v>0.3618273688942481</v>
       </c>
-    </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J23" s="2">
+        <f t="shared" si="3"/>
+        <v>0.13953621098603594</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>2011</v>
       </c>
@@ -2162,8 +3232,12 @@
         <f t="shared" si="2"/>
         <v>0.43454022001553017</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J24" s="2">
+        <f t="shared" si="3"/>
+        <v>9.2789552446865001E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>2012</v>
       </c>
@@ -2194,8 +3268,12 @@
         <f t="shared" si="2"/>
         <v>0.40209987908471057</v>
       </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J25" s="2">
+        <f t="shared" si="3"/>
+        <v>8.5652985219278763E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="8">
         <v>2013</v>
       </c>
@@ -2226,8 +3304,12 @@
         <f t="shared" si="2"/>
         <v>0.42696431913244037</v>
       </c>
-    </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J26" s="12">
+        <f t="shared" si="3"/>
+        <v>9.0822554345615064E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="8">
         <v>2014</v>
       </c>
@@ -2258,8 +3340,12 @@
         <f t="shared" si="2"/>
         <v>0.41602855319559939</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27" s="12">
+        <f t="shared" si="3"/>
+        <v>9.9265533835264139E-2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="8">
         <v>2015</v>
       </c>
@@ -2289,6 +3375,10 @@
       <c r="I28" s="12">
         <f t="shared" si="2"/>
         <v>0.45636985906238581</v>
+      </c>
+      <c r="J28" s="12">
+        <f t="shared" si="3"/>
+        <v>8.8456951293445982E-2</v>
       </c>
     </row>
   </sheetData>
@@ -2303,395 +3393,829 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S27"/>
+  <dimension ref="A1:AO27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="AG5" sqref="AG5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="BC2" sqref="BC2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="18.28515625" style="6" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.140625" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="6.28515625" style="6" customWidth="1"/>
+    <col min="39" max="39" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="34.5703125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>101</v>
-      </c>
-      <c r="R1" s="16" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" t="s">
+        <v>104</v>
+      </c>
+      <c r="S1" s="14" t="s">
         <v>1</v>
       </c>
-      <c r="S1" s="16" t="s">
+      <c r="T1" s="14" t="s">
         <v>103</v>
       </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL1" s="5" t="s">
+        <v>1</v>
+      </c>
+      <c r="AM1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="AN1" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="AO1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="6">
         <v>1990</v>
       </c>
       <c r="B2" s="7">
         <v>1.5687027579162412E-2</v>
       </c>
-      <c r="R2">
+      <c r="C2" s="7">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="S2">
         <v>1990</v>
       </c>
-      <c r="S2" s="2">
+      <c r="T2" s="2">
         <v>0.31291336079903176</v>
       </c>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL2" s="6">
+        <v>1990</v>
+      </c>
+      <c r="AM2" s="7">
+        <v>1.5687027579162412E-2</v>
+      </c>
+      <c r="AN2" s="7">
+        <v>4.5346288932896141E-2</v>
+      </c>
+      <c r="AO2" s="7">
+        <f>C2</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="6">
         <v>1991</v>
       </c>
       <c r="B3" s="7">
         <v>1.8284217618070749E-2</v>
       </c>
-      <c r="R3">
+      <c r="C3" s="7">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="S3">
         <v>1991</v>
       </c>
-      <c r="S3" s="2">
+      <c r="T3" s="2">
         <v>0.31696110663001692</v>
       </c>
-    </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL3" s="6">
+        <v>1991</v>
+      </c>
+      <c r="AM3" s="7">
+        <v>1.8284217618070749E-2</v>
+      </c>
+      <c r="AN3" s="7">
+        <v>5.221862614201879E-2</v>
+      </c>
+      <c r="AO3" s="7">
+        <f t="shared" ref="AO3:AO27" si="0">C3</f>
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="6">
         <v>1992</v>
       </c>
       <c r="B4" s="7">
         <v>1.7092164008498965E-2</v>
       </c>
-      <c r="R4">
+      <c r="C4" s="7">
+        <v>1.2500000000000001E-2</v>
+      </c>
+      <c r="S4">
         <v>1992</v>
       </c>
-      <c r="S4" s="2">
+      <c r="T4" s="2">
         <v>0.31870133940698325</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A5" s="17">
+      <c r="AL4" s="6">
+        <v>1992</v>
+      </c>
+      <c r="AM4" s="7">
+        <v>1.7092164008498965E-2</v>
+      </c>
+      <c r="AN4" s="7">
+        <v>4.8527854451927276E-2</v>
+      </c>
+      <c r="AO4" s="7">
+        <f t="shared" si="0"/>
+        <v>1.2500000000000001E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A5" s="15">
         <v>1993</v>
       </c>
-      <c r="B5" s="18">
+      <c r="B5" s="16">
         <v>2.3096859591647638E-2</v>
       </c>
-      <c r="R5" s="8">
+      <c r="C5" s="16">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S5" s="8">
         <v>1993</v>
       </c>
-      <c r="S5" s="12">
+      <c r="T5" s="12">
         <v>0.31870133940698325</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL5" s="15">
+        <v>1993</v>
+      </c>
+      <c r="AM5" s="16">
+        <v>2.3096859591647638E-2</v>
+      </c>
+      <c r="AN5" s="16">
+        <v>6.5700764877829623E-2</v>
+      </c>
+      <c r="AO5" s="16">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="6">
         <v>1994</v>
       </c>
       <c r="B6" s="7">
         <v>2.3564254028087435E-2</v>
       </c>
-      <c r="R6">
+      <c r="C6" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S6">
         <v>1994</v>
       </c>
-      <c r="S6" s="2">
+      <c r="T6" s="2">
         <v>0.29695819850537519</v>
       </c>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL6" s="6">
+        <v>1994</v>
+      </c>
+      <c r="AM6" s="7">
+        <v>2.3564254028087435E-2</v>
+      </c>
+      <c r="AN6" s="7">
+        <v>7.1988122820615633E-2</v>
+      </c>
+      <c r="AO6" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="6">
         <v>1995</v>
       </c>
       <c r="B7" s="7">
         <v>2.8593270957563973E-2</v>
       </c>
-      <c r="R7">
+      <c r="C7" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S7">
         <v>1995</v>
       </c>
-      <c r="S7" s="2">
+      <c r="T7" s="2">
         <v>0.31417322434052192</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL7" s="6">
+        <v>1995</v>
+      </c>
+      <c r="AM7" s="7">
+        <v>2.8593270957563973E-2</v>
+      </c>
+      <c r="AN7" s="7">
+        <v>8.2662367756665481E-2</v>
+      </c>
+      <c r="AO7" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="6">
         <v>1996</v>
       </c>
       <c r="B8" s="7">
         <v>3.0167446944406033E-2</v>
       </c>
-      <c r="R8">
+      <c r="C8" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S8">
         <v>1996</v>
       </c>
-      <c r="S8" s="2">
+      <c r="T8" s="2">
         <v>0.32517907384116584</v>
       </c>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL8" s="6">
+        <v>1996</v>
+      </c>
+      <c r="AM8" s="7">
+        <v>3.0167446944406033E-2</v>
+      </c>
+      <c r="AN8" s="7">
+        <v>8.4276464979243265E-2</v>
+      </c>
+      <c r="AO8" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="6">
         <v>1997</v>
       </c>
       <c r="B9" s="7">
         <v>3.5233025560722234E-2</v>
       </c>
-      <c r="R9">
+      <c r="C9" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S9">
         <v>1997</v>
       </c>
-      <c r="S9" s="2">
+      <c r="T9" s="2">
         <v>0.32281249471455076</v>
       </c>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL9" s="6">
+        <v>1997</v>
+      </c>
+      <c r="AM9" s="7">
+        <v>3.5233025560722234E-2</v>
+      </c>
+      <c r="AN9" s="7">
+        <v>9.9313486905973788E-2</v>
+      </c>
+      <c r="AO9" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A10" s="6">
         <v>1998</v>
       </c>
       <c r="B10" s="7">
         <v>3.5297669273030692E-2</v>
       </c>
-      <c r="R10">
+      <c r="C10" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S10">
         <v>1998</v>
       </c>
-      <c r="S10" s="2">
+      <c r="T10" s="2">
         <v>0.33640808016064533</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A11" s="17">
+      <c r="AL10" s="6">
+        <v>1998</v>
+      </c>
+      <c r="AM10" s="7">
+        <v>3.5297669273030692E-2</v>
+      </c>
+      <c r="AN10" s="7">
+        <v>9.5433980174787908E-2</v>
+      </c>
+      <c r="AO10" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A11" s="15">
         <v>1999</v>
       </c>
-      <c r="B11" s="18">
+      <c r="B11" s="16">
         <v>3.4372024061413653E-2</v>
       </c>
-      <c r="R11" s="8">
+      <c r="C11" s="16">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S11" s="8">
         <v>1999</v>
       </c>
-      <c r="S11" s="12">
+      <c r="T11" s="12">
         <v>0.33640808016064533</v>
       </c>
-    </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL11" s="15">
+        <v>1999</v>
+      </c>
+      <c r="AM11" s="16">
+        <v>3.4372024061413653E-2</v>
+      </c>
+      <c r="AN11" s="16">
+        <v>9.2905487302346657E-2</v>
+      </c>
+      <c r="AO11" s="16">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A12" s="6">
         <v>2000</v>
       </c>
       <c r="B12" s="7">
         <v>3.9052028113747105E-2</v>
       </c>
-      <c r="R12">
+      <c r="C12" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S12">
         <v>2000</v>
       </c>
-      <c r="S12" s="2">
+      <c r="T12" s="2">
         <v>0.30303721931421135</v>
       </c>
-    </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL12" s="6">
+        <v>2000</v>
+      </c>
+      <c r="AM12" s="7">
+        <v>3.9052028113747105E-2</v>
+      </c>
+      <c r="AN12" s="7">
+        <v>0.1174960330668553</v>
+      </c>
+      <c r="AO12" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A13" s="6">
         <v>2001</v>
       </c>
       <c r="B13" s="7">
         <v>4.8837151650157416E-2</v>
       </c>
-      <c r="R13">
+      <c r="C13" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S13">
         <v>2001</v>
       </c>
-      <c r="S13" s="2">
+      <c r="T13" s="2">
         <v>0.33893339454943977</v>
       </c>
-    </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL13" s="6">
+        <v>2001</v>
+      </c>
+      <c r="AM13" s="7">
+        <v>4.8837151650157416E-2</v>
+      </c>
+      <c r="AN13" s="7">
+        <v>0.13157754429262633</v>
+      </c>
+      <c r="AO13" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A14" s="6">
         <v>2002</v>
       </c>
       <c r="B14" s="7">
         <v>4.0877259972808007E-2</v>
       </c>
-      <c r="R14">
+      <c r="C14" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S14">
         <v>2002</v>
       </c>
-      <c r="S14" s="2">
+      <c r="T14" s="2">
         <v>0.29501687736228793</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL14" s="6">
+        <v>2002</v>
+      </c>
+      <c r="AM14" s="7">
+        <v>4.0877259972808007E-2</v>
+      </c>
+      <c r="AN14" s="7">
+        <v>0.12645530295920784</v>
+      </c>
+      <c r="AO14" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A15" s="6">
         <v>2003</v>
       </c>
       <c r="B15" s="7">
         <v>4.4030667534924864E-2</v>
       </c>
-      <c r="R15">
+      <c r="C15" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S15">
         <v>2003</v>
       </c>
-      <c r="S15" s="2">
+      <c r="T15" s="2">
         <v>0.32784927351810844</v>
       </c>
-    </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL15" s="6">
+        <v>2003</v>
+      </c>
+      <c r="AM15" s="7">
+        <v>4.4030667534924864E-2</v>
+      </c>
+      <c r="AN15" s="7">
+        <v>0.1225168202707379</v>
+      </c>
+      <c r="AO15" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A16" s="6">
         <v>2004</v>
       </c>
       <c r="B16" s="7">
         <v>4.4765475208358566E-2</v>
       </c>
-      <c r="R16">
+      <c r="C16" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S16">
         <v>2004</v>
       </c>
-      <c r="S16" s="2">
+      <c r="T16" s="2">
         <v>0.32311974698661361</v>
       </c>
-    </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL16" s="6">
+        <v>2004</v>
+      </c>
+      <c r="AM16" s="7">
+        <v>4.4765475208358566E-2</v>
+      </c>
+      <c r="AN16" s="7">
+        <v>0.12643900059712318</v>
+      </c>
+      <c r="AO16" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A17" s="6">
         <v>2005</v>
       </c>
       <c r="B17" s="7">
         <v>4.1536939381475367E-2</v>
       </c>
-      <c r="R17">
+      <c r="C17" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S17">
         <v>2005</v>
       </c>
-      <c r="S17" s="2">
+      <c r="T17" s="2">
         <v>0.34497296569717978</v>
       </c>
-    </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL17" s="6">
+        <v>2005</v>
+      </c>
+      <c r="AM17" s="7">
+        <v>4.1536939381475367E-2</v>
+      </c>
+      <c r="AN17" s="7">
+        <v>0.10968641899381416</v>
+      </c>
+      <c r="AO17" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A18" s="6">
         <v>2006</v>
       </c>
       <c r="B18" s="7">
         <v>4.0072430526595142E-2</v>
       </c>
-      <c r="R18">
+      <c r="C18" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S18">
         <v>2006</v>
       </c>
-      <c r="S18" s="2">
+      <c r="T18" s="2">
         <v>0.37183833435567315</v>
       </c>
-    </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL18" s="6">
+        <v>2006</v>
+      </c>
+      <c r="AM18" s="7">
+        <v>4.0072430526595142E-2</v>
+      </c>
+      <c r="AN18" s="7">
+        <v>9.8048230088917832E-2</v>
+      </c>
+      <c r="AO18" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A19" s="6">
         <v>2007</v>
       </c>
       <c r="B19" s="7">
         <v>3.7588499213079329E-2</v>
       </c>
-      <c r="R19">
+      <c r="C19" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S19">
         <v>2007</v>
       </c>
-      <c r="S19" s="2">
+      <c r="T19" s="2">
         <v>0.38686490932385847</v>
       </c>
-    </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL19" s="6">
+        <v>2007</v>
+      </c>
+      <c r="AM19" s="7">
+        <v>3.7588499213079329E-2</v>
+      </c>
+      <c r="AN19" s="7">
+        <v>8.8303613220131097E-2</v>
+      </c>
+      <c r="AO19" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A20" s="6">
         <v>2008</v>
       </c>
       <c r="B20" s="7">
         <v>3.7889508960268097E-2</v>
       </c>
-      <c r="R20">
+      <c r="C20" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S20">
         <v>2008</v>
       </c>
-      <c r="S20" s="2">
+      <c r="T20" s="2">
         <v>0.38033887264106064</v>
       </c>
-    </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL20" s="6">
+        <v>2008</v>
+      </c>
+      <c r="AM20" s="7">
+        <v>3.7889508960268097E-2</v>
+      </c>
+      <c r="AN20" s="7">
+        <v>9.0560523572040891E-2</v>
+      </c>
+      <c r="AO20" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A21" s="6">
         <v>2009</v>
       </c>
       <c r="B21" s="7">
         <v>5.1054109277875501E-2</v>
       </c>
-      <c r="R21">
+      <c r="C21" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S21">
         <v>2009</v>
       </c>
-      <c r="S21" s="2">
+      <c r="T21" s="2">
         <v>0.3777798937824654</v>
       </c>
-    </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL21" s="6">
+        <v>2009</v>
+      </c>
+      <c r="AM21" s="7">
+        <v>5.1054109277875501E-2</v>
+      </c>
+      <c r="AN21" s="7">
+        <v>0.12329445793584255</v>
+      </c>
+      <c r="AO21" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A22" s="6">
         <v>2010</v>
       </c>
       <c r="B22" s="7">
         <v>5.5241337110587443E-2</v>
       </c>
-      <c r="R22">
+      <c r="C22" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S22">
         <v>2010</v>
       </c>
-      <c r="S22" s="2">
+      <c r="T22" s="2">
         <v>0.3618273688942481</v>
       </c>
-    </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL22" s="6">
+        <v>2010</v>
+      </c>
+      <c r="AM22" s="7">
+        <v>5.5241337110587443E-2</v>
+      </c>
+      <c r="AN22" s="7">
+        <v>0.13953621098603594</v>
+      </c>
+      <c r="AO22" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A23" s="6">
         <v>2011</v>
       </c>
       <c r="B23" s="7">
         <v>4.4343699260644381E-2</v>
       </c>
-      <c r="R23">
+      <c r="C23" s="7">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="S23">
         <v>2011</v>
       </c>
-      <c r="S23" s="2">
+      <c r="T23" s="2">
         <v>0.43454022001553017</v>
       </c>
-    </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.25">
+      <c r="AL23" s="6">
+        <v>2011</v>
+      </c>
+      <c r="AM23" s="7">
+        <v>4.4343699260644381E-2</v>
+      </c>
+      <c r="AN23" s="7">
+        <v>9.2789552446865001E-2</v>
+      </c>
+      <c r="AO23" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A24" s="6">
         <v>2012</v>
       </c>
       <c r="B24" s="7">
         <v>3.7907077296420941E-2</v>
       </c>
-      <c r="R24">
+      <c r="C24" s="7">
+        <v>2.5999999999999999E-2</v>
+      </c>
+      <c r="S24">
         <v>2012</v>
       </c>
-      <c r="S24" s="2">
+      <c r="T24" s="2">
         <v>0.40209987908471057</v>
       </c>
-    </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A25" s="17">
+      <c r="AL24" s="6">
+        <v>2012</v>
+      </c>
+      <c r="AM24" s="7">
+        <v>3.7907077296420941E-2</v>
+      </c>
+      <c r="AN24" s="7">
+        <v>8.5652985219278763E-2</v>
+      </c>
+      <c r="AO24" s="7">
+        <f t="shared" si="0"/>
+        <v>2.5999999999999999E-2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A25" s="15">
         <v>2013</v>
       </c>
-      <c r="B25" s="18">
+      <c r="B25" s="16">
         <v>4.2656195131108195E-2</v>
       </c>
-      <c r="R25" s="8">
+      <c r="C25" s="16">
+        <v>2.7E-2</v>
+      </c>
+      <c r="S25" s="8">
         <v>2013</v>
       </c>
-      <c r="S25" s="12">
+      <c r="T25" s="12">
         <v>0.42696431913244037</v>
       </c>
-    </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
+      <c r="AL25" s="15">
+        <v>2013</v>
+      </c>
+      <c r="AM25" s="16">
+        <v>4.2656195131108195E-2</v>
+      </c>
+      <c r="AN25" s="16">
+        <v>9.0822554345615064E-2</v>
+      </c>
+      <c r="AO25" s="16">
+        <f t="shared" si="0"/>
+        <v>2.7E-2</v>
+      </c>
+    </row>
+    <row r="26" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A26" s="15">
         <v>2014</v>
       </c>
-      <c r="B26" s="18">
+      <c r="B26" s="16">
         <v>4.5385307495546069E-2</v>
       </c>
-      <c r="R26" s="8">
+      <c r="C26" s="16">
+        <v>2.8000000000000001E-2</v>
+      </c>
+      <c r="S26" s="8">
         <v>2014</v>
       </c>
-      <c r="S26" s="12">
+      <c r="T26" s="12">
         <v>0.41602855319559939</v>
       </c>
-    </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A27" s="17">
+      <c r="AL26" s="15">
+        <v>2014</v>
+      </c>
+      <c r="AM26" s="16">
+        <v>4.5385307495546069E-2</v>
+      </c>
+      <c r="AN26" s="16">
+        <v>9.9265533835264139E-2</v>
+      </c>
+      <c r="AO26" s="16">
+        <f t="shared" si="0"/>
+        <v>2.8000000000000001E-2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
+      <c r="A27" s="15">
         <v>2015</v>
       </c>
-      <c r="B27" s="18">
+      <c r="B27" s="16">
         <v>4.4417976133047585E-2</v>
       </c>
-      <c r="R27" s="8">
+      <c r="C27" s="16">
+        <v>2.9000000000000001E-2</v>
+      </c>
+      <c r="S27" s="8">
         <v>2015</v>
       </c>
-      <c r="S27" s="12">
+      <c r="T27" s="12">
         <v>0.45636985906238581</v>
+      </c>
+      <c r="AL27" s="15">
+        <v>2015</v>
+      </c>
+      <c r="AM27" s="16">
+        <v>4.4417976133047585E-2</v>
+      </c>
+      <c r="AN27" s="16">
+        <v>8.8456951293445982E-2</v>
+      </c>
+      <c r="AO27" s="16">
+        <f t="shared" si="0"/>
+        <v>2.9000000000000001E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Modified presentation for FinalProject
</commit_message>
<xml_diff>
--- a/FinalProject/Docs/Townes_POLS6310_2019_Spring_FinalProject_Charts_v00.xlsx
+++ b/FinalProject/Docs/Townes_POLS6310_2019_Spring_FinalProject_Charts_v00.xlsx
@@ -908,11 +908,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="159665152"/>
-        <c:axId val="159671040"/>
+        <c:axId val="161129216"/>
+        <c:axId val="161130752"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="159665152"/>
+        <c:axId val="161129216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2015"/>
@@ -924,13 +924,13 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159671040"/>
+        <c:crossAx val="161130752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="159671040"/>
+        <c:axId val="161130752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -941,11 +941,16 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159665152"/>
+        <c:crossAx val="161129216"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -988,11 +993,19 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Small Business </a:t>
+              <a:t>Utilization Efficiency</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Federally-Funded R&amp;D Percentage of Potential</a:t>
+              <a:t> of </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Small Business for </a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t>Federally-Funded R&amp;D</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1205,11 +1218,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="159699328"/>
-        <c:axId val="159700864"/>
+        <c:axId val="161146752"/>
+        <c:axId val="161148288"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="159699328"/>
+        <c:axId val="161146752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2015"/>
@@ -1221,12 +1234,12 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159700864"/>
+        <c:crossAx val="161148288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="159700864"/>
+        <c:axId val="161148288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1237,7 +1250,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="159699328"/>
+        <c:crossAx val="161146752"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1284,11 +1297,11 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="en-US"/>
-              <a:t>Targets for Small</a:t>
+              <a:t>Small</a:t>
             </a:r>
             <a:r>
               <a:rPr lang="en-US" baseline="0"/>
-              <a:t> Business R&amp;D Funding</a:t>
+              <a:t> Business Participation in Federally Funded R&amp;D</a:t>
             </a:r>
             <a:endParaRPr lang="en-US"/>
           </a:p>
@@ -1645,82 +1658,82 @@
                 <c:formatCode>0.00%</c:formatCode>
                 <c:ptCount val="26"/>
                 <c:pt idx="0">
-                  <c:v>4.5346288932896141E-2</c:v>
+                  <c:v>2.5710550768848112E-2</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>5.221862614201879E-2</c:v>
+                  <c:v>2.9699625019090455E-2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>4.8527854451927276E-2</c:v>
+                  <c:v>2.7554206482956603E-2</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>6.5700764877829623E-2</c:v>
+                  <c:v>3.7598308316348257E-2</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.1988122820615633E-2</c:v>
+                  <c:v>4.1315272184054404E-2</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>8.2662367756665481E-2</c:v>
+                  <c:v>4.7675063708869737E-2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>8.4276464979243265E-2</c:v>
+                  <c:v>4.8642211030432578E-2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.9313486905973788E-2</c:v>
+                  <c:v>5.7721968253696798E-2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.5433980174787908E-2</c:v>
+                  <c:v>5.5367287017810858E-2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9.2905487302346657E-2</c:v>
+                  <c:v>5.3837167747786491E-2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.1174960330668553</c:v>
+                  <c:v>6.8872106974220498E-2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.13157754429262633</c:v>
+                  <c:v>7.7638872229034789E-2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.12645530295920784</c:v>
+                  <c:v>7.4436450016466676E-2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.1225168202707379</c:v>
+                  <c:v>7.1984599830261092E-2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.12643900059712318</c:v>
+                  <c:v>7.4426282452373926E-2</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.10968641899381416</c:v>
+                  <c:v>6.4059783089266603E-2</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.8048230088917832E-2</c:v>
+                  <c:v>5.6953082929089745E-2</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>8.8303613220131097E-2</c:v>
+                  <c:v>5.1061526123744261E-2</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.0560523572040891E-2</c:v>
+                  <c:v>5.2421313818112741E-2</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.12329445793584255</c:v>
+                  <c:v>7.2467988337594602E-2</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.13953621098603594</c:v>
+                  <c:v>8.2645466195862244E-2</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.2789552446865001E-2</c:v>
+                  <c:v>5.3767095690706534E-2</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>8.5652985219278763E-2</c:v>
+                  <c:v>4.9468144799758806E-2</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.0822554345615064E-2</c:v>
+                  <c:v>5.2579371445597739E-2</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>9.9265533835264139E-2</c:v>
+                  <c:v>5.7692811105290613E-2</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.8456951293445982E-2</c:v>
+                  <c:v>5.1153822350645375E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1944,11 +1957,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="164856192"/>
-        <c:axId val="164854400"/>
+        <c:axId val="161304960"/>
+        <c:axId val="161306880"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="164856192"/>
+        <c:axId val="161304960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2015"/>
@@ -1960,12 +1973,12 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164854400"/>
+        <c:crossAx val="161306880"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="164854400"/>
+        <c:axId val="161306880"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1973,12 +1986,13 @@
         <c:axPos val="l"/>
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
+        <c:majorTickMark val="cross"/>
+        <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="164856192"/>
+        <c:crossAx val="161304960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:minorUnit val="1.0000000000000002E-2"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
@@ -2073,10 +2087,10 @@
       <xdr:rowOff>71436</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>53</xdr:col>
-      <xdr:colOff>523875</xdr:colOff>
+      <xdr:col>54</xdr:col>
+      <xdr:colOff>571501</xdr:colOff>
       <xdr:row>26</xdr:row>
-      <xdr:rowOff>114299</xdr:rowOff>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -2388,7 +2402,7 @@
   <dimension ref="A1:J28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J28"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2477,8 +2491,8 @@
         <v>0.31291336079903176</v>
       </c>
       <c r="J3" s="2">
-        <f>(($D3/0.15)+($E3/0.5))/(($D3/0.15)+($E3/0.5)+(($F3-(($D3/0.15)+($E3/0.5)))/0.9))</f>
-        <v>4.5346288932896141E-2</v>
+        <f>(($D3/0.15)+($E3/0.5))/(($D3/0.15)+($E3/0.5)+(($F3-(($D3/0.15)+($E3/0.5)))/0.5))</f>
+        <v>2.5710550768848112E-2</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
@@ -2513,8 +2527,8 @@
         <v>0.31696110663001692</v>
       </c>
       <c r="J4" s="2">
-        <f t="shared" ref="J4:J28" si="3">(($D4/0.15)+($E4/0.5))/(($D4/0.15)+($E4/0.5)+(($F4-(($D4/0.15)+($E4/0.5)))/0.9))</f>
-        <v>5.221862614201879E-2</v>
+        <f t="shared" ref="J4:J28" si="3">(($D4/0.15)+($E4/0.5))/(($D4/0.15)+($E4/0.5)+(($F4-(($D4/0.15)+($E4/0.5)))/0.5))</f>
+        <v>2.9699625019090455E-2</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -2550,7 +2564,7 @@
       </c>
       <c r="J5" s="2">
         <f t="shared" si="3"/>
-        <v>4.8527854451927276E-2</v>
+        <v>2.7554206482956603E-2</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
@@ -2586,7 +2600,7 @@
       </c>
       <c r="J6" s="12">
         <f t="shared" si="3"/>
-        <v>6.5700764877829623E-2</v>
+        <v>3.7598308316348257E-2</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
@@ -2622,7 +2636,7 @@
       </c>
       <c r="J7" s="2">
         <f t="shared" si="3"/>
-        <v>7.1988122820615633E-2</v>
+        <v>4.1315272184054404E-2</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
@@ -2658,7 +2672,7 @@
       </c>
       <c r="J8" s="2">
         <f t="shared" si="3"/>
-        <v>8.2662367756665481E-2</v>
+        <v>4.7675063708869737E-2</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
@@ -2694,7 +2708,7 @@
       </c>
       <c r="J9" s="2">
         <f t="shared" si="3"/>
-        <v>8.4276464979243265E-2</v>
+        <v>4.8642211030432578E-2</v>
       </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
@@ -2730,7 +2744,7 @@
       </c>
       <c r="J10" s="2">
         <f t="shared" si="3"/>
-        <v>9.9313486905973788E-2</v>
+        <v>5.7721968253696798E-2</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
@@ -2766,7 +2780,7 @@
       </c>
       <c r="J11" s="2">
         <f t="shared" si="3"/>
-        <v>9.5433980174787908E-2</v>
+        <v>5.5367287017810858E-2</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
@@ -2802,7 +2816,7 @@
       </c>
       <c r="J12" s="12">
         <f t="shared" si="3"/>
-        <v>9.2905487302346657E-2</v>
+        <v>5.3837167747786491E-2</v>
       </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
@@ -2838,7 +2852,7 @@
       </c>
       <c r="J13" s="2">
         <f t="shared" si="3"/>
-        <v>0.1174960330668553</v>
+        <v>6.8872106974220498E-2</v>
       </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
@@ -2874,7 +2888,7 @@
       </c>
       <c r="J14" s="2">
         <f t="shared" si="3"/>
-        <v>0.13157754429262633</v>
+        <v>7.7638872229034789E-2</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
@@ -2910,7 +2924,7 @@
       </c>
       <c r="J15" s="2">
         <f t="shared" si="3"/>
-        <v>0.12645530295920784</v>
+        <v>7.4436450016466676E-2</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
@@ -2946,7 +2960,7 @@
       </c>
       <c r="J16" s="2">
         <f t="shared" si="3"/>
-        <v>0.1225168202707379</v>
+        <v>7.1984599830261092E-2</v>
       </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
@@ -2982,7 +2996,7 @@
       </c>
       <c r="J17" s="2">
         <f t="shared" si="3"/>
-        <v>0.12643900059712318</v>
+        <v>7.4426282452373926E-2</v>
       </c>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
@@ -3018,7 +3032,7 @@
       </c>
       <c r="J18" s="2">
         <f t="shared" si="3"/>
-        <v>0.10968641899381416</v>
+        <v>6.4059783089266603E-2</v>
       </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
@@ -3054,7 +3068,7 @@
       </c>
       <c r="J19" s="2">
         <f t="shared" si="3"/>
-        <v>9.8048230088917832E-2</v>
+        <v>5.6953082929089745E-2</v>
       </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
@@ -3090,7 +3104,7 @@
       </c>
       <c r="J20" s="2">
         <f t="shared" si="3"/>
-        <v>8.8303613220131097E-2</v>
+        <v>5.1061526123744261E-2</v>
       </c>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
@@ -3126,7 +3140,7 @@
       </c>
       <c r="J21" s="2">
         <f t="shared" si="3"/>
-        <v>9.0560523572040891E-2</v>
+        <v>5.2421313818112741E-2</v>
       </c>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
@@ -3162,7 +3176,7 @@
       </c>
       <c r="J22" s="2">
         <f t="shared" si="3"/>
-        <v>0.12329445793584255</v>
+        <v>7.2467988337594602E-2</v>
       </c>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
@@ -3198,7 +3212,7 @@
       </c>
       <c r="J23" s="2">
         <f t="shared" si="3"/>
-        <v>0.13953621098603594</v>
+        <v>8.2645466195862244E-2</v>
       </c>
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
@@ -3234,7 +3248,7 @@
       </c>
       <c r="J24" s="2">
         <f t="shared" si="3"/>
-        <v>9.2789552446865001E-2</v>
+        <v>5.3767095690706534E-2</v>
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
@@ -3270,7 +3284,7 @@
       </c>
       <c r="J25" s="2">
         <f t="shared" si="3"/>
-        <v>8.5652985219278763E-2</v>
+        <v>4.9468144799758806E-2</v>
       </c>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
@@ -3306,7 +3320,7 @@
       </c>
       <c r="J26" s="12">
         <f t="shared" si="3"/>
-        <v>9.0822554345615064E-2</v>
+        <v>5.2579371445597739E-2</v>
       </c>
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
@@ -3342,7 +3356,7 @@
       </c>
       <c r="J27" s="12">
         <f t="shared" si="3"/>
-        <v>9.9265533835264139E-2</v>
+        <v>5.7692811105290613E-2</v>
       </c>
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
@@ -3378,7 +3392,7 @@
       </c>
       <c r="J28" s="12">
         <f t="shared" si="3"/>
-        <v>8.8456951293445982E-2</v>
+        <v>5.1153822350645375E-2</v>
       </c>
     </row>
   </sheetData>
@@ -3395,8 +3409,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="BC2" sqref="BC2"/>
+    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
+      <selection activeCell="BD2" sqref="BD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3443,6 +3457,7 @@
         <v>1990</v>
       </c>
       <c r="B2" s="7">
+        <f>DataRaw!G3</f>
         <v>1.5687027579162412E-2</v>
       </c>
       <c r="C2" s="7">
@@ -3452,16 +3467,19 @@
         <v>1990</v>
       </c>
       <c r="T2" s="2">
+        <f>DataRaw!I3</f>
         <v>0.31291336079903176</v>
       </c>
       <c r="AL2" s="6">
         <v>1990</v>
       </c>
       <c r="AM2" s="7">
+        <f>DataRaw!G3</f>
         <v>1.5687027579162412E-2</v>
       </c>
       <c r="AN2" s="7">
-        <v>4.5346288932896141E-2</v>
+        <f>DataRaw!J3</f>
+        <v>2.5710550768848112E-2</v>
       </c>
       <c r="AO2" s="7">
         <f>C2</f>
@@ -3473,6 +3491,7 @@
         <v>1991</v>
       </c>
       <c r="B3" s="7">
+        <f>DataRaw!G4</f>
         <v>1.8284217618070749E-2</v>
       </c>
       <c r="C3" s="7">
@@ -3482,16 +3501,19 @@
         <v>1991</v>
       </c>
       <c r="T3" s="2">
+        <f>DataRaw!I4</f>
         <v>0.31696110663001692</v>
       </c>
       <c r="AL3" s="6">
         <v>1991</v>
       </c>
       <c r="AM3" s="7">
+        <f>DataRaw!G4</f>
         <v>1.8284217618070749E-2</v>
       </c>
       <c r="AN3" s="7">
-        <v>5.221862614201879E-2</v>
+        <f>DataRaw!J4</f>
+        <v>2.9699625019090455E-2</v>
       </c>
       <c r="AO3" s="7">
         <f t="shared" ref="AO3:AO27" si="0">C3</f>
@@ -3503,6 +3525,7 @@
         <v>1992</v>
       </c>
       <c r="B4" s="7">
+        <f>DataRaw!G5</f>
         <v>1.7092164008498965E-2</v>
       </c>
       <c r="C4" s="7">
@@ -3512,16 +3535,19 @@
         <v>1992</v>
       </c>
       <c r="T4" s="2">
+        <f>DataRaw!I5</f>
         <v>0.31870133940698325</v>
       </c>
       <c r="AL4" s="6">
         <v>1992</v>
       </c>
       <c r="AM4" s="7">
+        <f>DataRaw!G5</f>
         <v>1.7092164008498965E-2</v>
       </c>
       <c r="AN4" s="7">
-        <v>4.8527854451927276E-2</v>
+        <f>DataRaw!J5</f>
+        <v>2.7554206482956603E-2</v>
       </c>
       <c r="AO4" s="7">
         <f t="shared" si="0"/>
@@ -3533,6 +3559,7 @@
         <v>1993</v>
       </c>
       <c r="B5" s="16">
+        <f>DataRaw!G6</f>
         <v>2.3096859591647638E-2</v>
       </c>
       <c r="C5" s="16">
@@ -3542,16 +3569,19 @@
         <v>1993</v>
       </c>
       <c r="T5" s="12">
+        <f>DataRaw!I6</f>
         <v>0.31870133940698325</v>
       </c>
       <c r="AL5" s="15">
         <v>1993</v>
       </c>
       <c r="AM5" s="16">
+        <f>DataRaw!G6</f>
         <v>2.3096859591647638E-2</v>
       </c>
       <c r="AN5" s="16">
-        <v>6.5700764877829623E-2</v>
+        <f>DataRaw!J6</f>
+        <v>3.7598308316348257E-2</v>
       </c>
       <c r="AO5" s="16">
         <f t="shared" si="0"/>
@@ -3563,6 +3593,7 @@
         <v>1994</v>
       </c>
       <c r="B6" s="7">
+        <f>DataRaw!G7</f>
         <v>2.3564254028087435E-2</v>
       </c>
       <c r="C6" s="7">
@@ -3572,16 +3603,19 @@
         <v>1994</v>
       </c>
       <c r="T6" s="2">
+        <f>DataRaw!I7</f>
         <v>0.29695819850537519</v>
       </c>
       <c r="AL6" s="6">
         <v>1994</v>
       </c>
       <c r="AM6" s="7">
+        <f>DataRaw!G7</f>
         <v>2.3564254028087435E-2</v>
       </c>
       <c r="AN6" s="7">
-        <v>7.1988122820615633E-2</v>
+        <f>DataRaw!J7</f>
+        <v>4.1315272184054404E-2</v>
       </c>
       <c r="AO6" s="7">
         <f t="shared" si="0"/>
@@ -3593,6 +3627,7 @@
         <v>1995</v>
       </c>
       <c r="B7" s="7">
+        <f>DataRaw!G8</f>
         <v>2.8593270957563973E-2</v>
       </c>
       <c r="C7" s="7">
@@ -3602,16 +3637,19 @@
         <v>1995</v>
       </c>
       <c r="T7" s="2">
+        <f>DataRaw!I8</f>
         <v>0.31417322434052192</v>
       </c>
       <c r="AL7" s="6">
         <v>1995</v>
       </c>
       <c r="AM7" s="7">
+        <f>DataRaw!G8</f>
         <v>2.8593270957563973E-2</v>
       </c>
       <c r="AN7" s="7">
-        <v>8.2662367756665481E-2</v>
+        <f>DataRaw!J8</f>
+        <v>4.7675063708869737E-2</v>
       </c>
       <c r="AO7" s="7">
         <f t="shared" si="0"/>
@@ -3623,6 +3661,7 @@
         <v>1996</v>
       </c>
       <c r="B8" s="7">
+        <f>DataRaw!G9</f>
         <v>3.0167446944406033E-2</v>
       </c>
       <c r="C8" s="7">
@@ -3632,16 +3671,19 @@
         <v>1996</v>
       </c>
       <c r="T8" s="2">
+        <f>DataRaw!I9</f>
         <v>0.32517907384116584</v>
       </c>
       <c r="AL8" s="6">
         <v>1996</v>
       </c>
       <c r="AM8" s="7">
+        <f>DataRaw!G9</f>
         <v>3.0167446944406033E-2</v>
       </c>
       <c r="AN8" s="7">
-        <v>8.4276464979243265E-2</v>
+        <f>DataRaw!J9</f>
+        <v>4.8642211030432578E-2</v>
       </c>
       <c r="AO8" s="7">
         <f t="shared" si="0"/>
@@ -3653,6 +3695,7 @@
         <v>1997</v>
       </c>
       <c r="B9" s="7">
+        <f>DataRaw!G10</f>
         <v>3.5233025560722234E-2</v>
       </c>
       <c r="C9" s="7">
@@ -3662,16 +3705,19 @@
         <v>1997</v>
       </c>
       <c r="T9" s="2">
+        <f>DataRaw!I10</f>
         <v>0.32281249471455076</v>
       </c>
       <c r="AL9" s="6">
         <v>1997</v>
       </c>
       <c r="AM9" s="7">
+        <f>DataRaw!G10</f>
         <v>3.5233025560722234E-2</v>
       </c>
       <c r="AN9" s="7">
-        <v>9.9313486905973788E-2</v>
+        <f>DataRaw!J10</f>
+        <v>5.7721968253696798E-2</v>
       </c>
       <c r="AO9" s="7">
         <f t="shared" si="0"/>
@@ -3683,6 +3729,7 @@
         <v>1998</v>
       </c>
       <c r="B10" s="7">
+        <f>DataRaw!G11</f>
         <v>3.5297669273030692E-2</v>
       </c>
       <c r="C10" s="7">
@@ -3692,16 +3739,19 @@
         <v>1998</v>
       </c>
       <c r="T10" s="2">
+        <f>DataRaw!I11</f>
         <v>0.33640808016064533</v>
       </c>
       <c r="AL10" s="6">
         <v>1998</v>
       </c>
       <c r="AM10" s="7">
+        <f>DataRaw!G11</f>
         <v>3.5297669273030692E-2</v>
       </c>
       <c r="AN10" s="7">
-        <v>9.5433980174787908E-2</v>
+        <f>DataRaw!J11</f>
+        <v>5.5367287017810858E-2</v>
       </c>
       <c r="AO10" s="7">
         <f t="shared" si="0"/>
@@ -3713,6 +3763,7 @@
         <v>1999</v>
       </c>
       <c r="B11" s="16">
+        <f>DataRaw!G12</f>
         <v>3.4372024061413653E-2</v>
       </c>
       <c r="C11" s="16">
@@ -3722,16 +3773,19 @@
         <v>1999</v>
       </c>
       <c r="T11" s="12">
+        <f>DataRaw!I12</f>
         <v>0.33640808016064533</v>
       </c>
       <c r="AL11" s="15">
         <v>1999</v>
       </c>
       <c r="AM11" s="16">
+        <f>DataRaw!G12</f>
         <v>3.4372024061413653E-2</v>
       </c>
       <c r="AN11" s="16">
-        <v>9.2905487302346657E-2</v>
+        <f>DataRaw!J12</f>
+        <v>5.3837167747786491E-2</v>
       </c>
       <c r="AO11" s="16">
         <f t="shared" si="0"/>
@@ -3743,6 +3797,7 @@
         <v>2000</v>
       </c>
       <c r="B12" s="7">
+        <f>DataRaw!G13</f>
         <v>3.9052028113747105E-2</v>
       </c>
       <c r="C12" s="7">
@@ -3752,16 +3807,19 @@
         <v>2000</v>
       </c>
       <c r="T12" s="2">
+        <f>DataRaw!I13</f>
         <v>0.30303721931421135</v>
       </c>
       <c r="AL12" s="6">
         <v>2000</v>
       </c>
       <c r="AM12" s="7">
+        <f>DataRaw!G13</f>
         <v>3.9052028113747105E-2</v>
       </c>
       <c r="AN12" s="7">
-        <v>0.1174960330668553</v>
+        <f>DataRaw!J13</f>
+        <v>6.8872106974220498E-2</v>
       </c>
       <c r="AO12" s="7">
         <f t="shared" si="0"/>
@@ -3773,6 +3831,7 @@
         <v>2001</v>
       </c>
       <c r="B13" s="7">
+        <f>DataRaw!G14</f>
         <v>4.8837151650157416E-2</v>
       </c>
       <c r="C13" s="7">
@@ -3782,16 +3841,19 @@
         <v>2001</v>
       </c>
       <c r="T13" s="2">
+        <f>DataRaw!I14</f>
         <v>0.33893339454943977</v>
       </c>
       <c r="AL13" s="6">
         <v>2001</v>
       </c>
       <c r="AM13" s="7">
+        <f>DataRaw!G14</f>
         <v>4.8837151650157416E-2</v>
       </c>
       <c r="AN13" s="7">
-        <v>0.13157754429262633</v>
+        <f>DataRaw!J14</f>
+        <v>7.7638872229034789E-2</v>
       </c>
       <c r="AO13" s="7">
         <f t="shared" si="0"/>
@@ -3803,6 +3865,7 @@
         <v>2002</v>
       </c>
       <c r="B14" s="7">
+        <f>DataRaw!G15</f>
         <v>4.0877259972808007E-2</v>
       </c>
       <c r="C14" s="7">
@@ -3812,16 +3875,19 @@
         <v>2002</v>
       </c>
       <c r="T14" s="2">
+        <f>DataRaw!I15</f>
         <v>0.29501687736228793</v>
       </c>
       <c r="AL14" s="6">
         <v>2002</v>
       </c>
       <c r="AM14" s="7">
+        <f>DataRaw!G15</f>
         <v>4.0877259972808007E-2</v>
       </c>
       <c r="AN14" s="7">
-        <v>0.12645530295920784</v>
+        <f>DataRaw!J15</f>
+        <v>7.4436450016466676E-2</v>
       </c>
       <c r="AO14" s="7">
         <f t="shared" si="0"/>
@@ -3833,6 +3899,7 @@
         <v>2003</v>
       </c>
       <c r="B15" s="7">
+        <f>DataRaw!G16</f>
         <v>4.4030667534924864E-2</v>
       </c>
       <c r="C15" s="7">
@@ -3842,16 +3909,19 @@
         <v>2003</v>
       </c>
       <c r="T15" s="2">
+        <f>DataRaw!I16</f>
         <v>0.32784927351810844</v>
       </c>
       <c r="AL15" s="6">
         <v>2003</v>
       </c>
       <c r="AM15" s="7">
+        <f>DataRaw!G16</f>
         <v>4.4030667534924864E-2</v>
       </c>
       <c r="AN15" s="7">
-        <v>0.1225168202707379</v>
+        <f>DataRaw!J16</f>
+        <v>7.1984599830261092E-2</v>
       </c>
       <c r="AO15" s="7">
         <f t="shared" si="0"/>
@@ -3863,6 +3933,7 @@
         <v>2004</v>
       </c>
       <c r="B16" s="7">
+        <f>DataRaw!G17</f>
         <v>4.4765475208358566E-2</v>
       </c>
       <c r="C16" s="7">
@@ -3872,16 +3943,19 @@
         <v>2004</v>
       </c>
       <c r="T16" s="2">
+        <f>DataRaw!I17</f>
         <v>0.32311974698661361</v>
       </c>
       <c r="AL16" s="6">
         <v>2004</v>
       </c>
       <c r="AM16" s="7">
+        <f>DataRaw!G17</f>
         <v>4.4765475208358566E-2</v>
       </c>
       <c r="AN16" s="7">
-        <v>0.12643900059712318</v>
+        <f>DataRaw!J17</f>
+        <v>7.4426282452373926E-2</v>
       </c>
       <c r="AO16" s="7">
         <f t="shared" si="0"/>
@@ -3893,6 +3967,7 @@
         <v>2005</v>
       </c>
       <c r="B17" s="7">
+        <f>DataRaw!G18</f>
         <v>4.1536939381475367E-2</v>
       </c>
       <c r="C17" s="7">
@@ -3902,16 +3977,19 @@
         <v>2005</v>
       </c>
       <c r="T17" s="2">
+        <f>DataRaw!I18</f>
         <v>0.34497296569717978</v>
       </c>
       <c r="AL17" s="6">
         <v>2005</v>
       </c>
       <c r="AM17" s="7">
+        <f>DataRaw!G18</f>
         <v>4.1536939381475367E-2</v>
       </c>
       <c r="AN17" s="7">
-        <v>0.10968641899381416</v>
+        <f>DataRaw!J18</f>
+        <v>6.4059783089266603E-2</v>
       </c>
       <c r="AO17" s="7">
         <f t="shared" si="0"/>
@@ -3923,6 +4001,7 @@
         <v>2006</v>
       </c>
       <c r="B18" s="7">
+        <f>DataRaw!G19</f>
         <v>4.0072430526595142E-2</v>
       </c>
       <c r="C18" s="7">
@@ -3932,16 +4011,19 @@
         <v>2006</v>
       </c>
       <c r="T18" s="2">
+        <f>DataRaw!I19</f>
         <v>0.37183833435567315</v>
       </c>
       <c r="AL18" s="6">
         <v>2006</v>
       </c>
       <c r="AM18" s="7">
+        <f>DataRaw!G19</f>
         <v>4.0072430526595142E-2</v>
       </c>
       <c r="AN18" s="7">
-        <v>9.8048230088917832E-2</v>
+        <f>DataRaw!J19</f>
+        <v>5.6953082929089745E-2</v>
       </c>
       <c r="AO18" s="7">
         <f t="shared" si="0"/>
@@ -3953,6 +4035,7 @@
         <v>2007</v>
       </c>
       <c r="B19" s="7">
+        <f>DataRaw!G20</f>
         <v>3.7588499213079329E-2</v>
       </c>
       <c r="C19" s="7">
@@ -3962,16 +4045,19 @@
         <v>2007</v>
       </c>
       <c r="T19" s="2">
+        <f>DataRaw!I20</f>
         <v>0.38686490932385847</v>
       </c>
       <c r="AL19" s="6">
         <v>2007</v>
       </c>
       <c r="AM19" s="7">
+        <f>DataRaw!G20</f>
         <v>3.7588499213079329E-2</v>
       </c>
       <c r="AN19" s="7">
-        <v>8.8303613220131097E-2</v>
+        <f>DataRaw!J20</f>
+        <v>5.1061526123744261E-2</v>
       </c>
       <c r="AO19" s="7">
         <f t="shared" si="0"/>
@@ -3983,6 +4069,7 @@
         <v>2008</v>
       </c>
       <c r="B20" s="7">
+        <f>DataRaw!G21</f>
         <v>3.7889508960268097E-2</v>
       </c>
       <c r="C20" s="7">
@@ -3992,16 +4079,19 @@
         <v>2008</v>
       </c>
       <c r="T20" s="2">
+        <f>DataRaw!I21</f>
         <v>0.38033887264106064</v>
       </c>
       <c r="AL20" s="6">
         <v>2008</v>
       </c>
       <c r="AM20" s="7">
+        <f>DataRaw!G21</f>
         <v>3.7889508960268097E-2</v>
       </c>
       <c r="AN20" s="7">
-        <v>9.0560523572040891E-2</v>
+        <f>DataRaw!J21</f>
+        <v>5.2421313818112741E-2</v>
       </c>
       <c r="AO20" s="7">
         <f t="shared" si="0"/>
@@ -4013,6 +4103,7 @@
         <v>2009</v>
       </c>
       <c r="B21" s="7">
+        <f>DataRaw!G22</f>
         <v>5.1054109277875501E-2</v>
       </c>
       <c r="C21" s="7">
@@ -4022,16 +4113,19 @@
         <v>2009</v>
       </c>
       <c r="T21" s="2">
+        <f>DataRaw!I22</f>
         <v>0.3777798937824654</v>
       </c>
       <c r="AL21" s="6">
         <v>2009</v>
       </c>
       <c r="AM21" s="7">
+        <f>DataRaw!G22</f>
         <v>5.1054109277875501E-2</v>
       </c>
       <c r="AN21" s="7">
-        <v>0.12329445793584255</v>
+        <f>DataRaw!J22</f>
+        <v>7.2467988337594602E-2</v>
       </c>
       <c r="AO21" s="7">
         <f t="shared" si="0"/>
@@ -4043,6 +4137,7 @@
         <v>2010</v>
       </c>
       <c r="B22" s="7">
+        <f>DataRaw!G23</f>
         <v>5.5241337110587443E-2</v>
       </c>
       <c r="C22" s="7">
@@ -4052,16 +4147,19 @@
         <v>2010</v>
       </c>
       <c r="T22" s="2">
+        <f>DataRaw!I23</f>
         <v>0.3618273688942481</v>
       </c>
       <c r="AL22" s="6">
         <v>2010</v>
       </c>
       <c r="AM22" s="7">
+        <f>DataRaw!G23</f>
         <v>5.5241337110587443E-2</v>
       </c>
       <c r="AN22" s="7">
-        <v>0.13953621098603594</v>
+        <f>DataRaw!J23</f>
+        <v>8.2645466195862244E-2</v>
       </c>
       <c r="AO22" s="7">
         <f t="shared" si="0"/>
@@ -4073,6 +4171,7 @@
         <v>2011</v>
       </c>
       <c r="B23" s="7">
+        <f>DataRaw!G24</f>
         <v>4.4343699260644381E-2</v>
       </c>
       <c r="C23" s="7">
@@ -4082,16 +4181,19 @@
         <v>2011</v>
       </c>
       <c r="T23" s="2">
+        <f>DataRaw!I24</f>
         <v>0.43454022001553017</v>
       </c>
       <c r="AL23" s="6">
         <v>2011</v>
       </c>
       <c r="AM23" s="7">
+        <f>DataRaw!G24</f>
         <v>4.4343699260644381E-2</v>
       </c>
       <c r="AN23" s="7">
-        <v>9.2789552446865001E-2</v>
+        <f>DataRaw!J24</f>
+        <v>5.3767095690706534E-2</v>
       </c>
       <c r="AO23" s="7">
         <f t="shared" si="0"/>
@@ -4103,6 +4205,7 @@
         <v>2012</v>
       </c>
       <c r="B24" s="7">
+        <f>DataRaw!G25</f>
         <v>3.7907077296420941E-2</v>
       </c>
       <c r="C24" s="7">
@@ -4112,16 +4215,19 @@
         <v>2012</v>
       </c>
       <c r="T24" s="2">
+        <f>DataRaw!I25</f>
         <v>0.40209987908471057</v>
       </c>
       <c r="AL24" s="6">
         <v>2012</v>
       </c>
       <c r="AM24" s="7">
+        <f>DataRaw!G25</f>
         <v>3.7907077296420941E-2</v>
       </c>
       <c r="AN24" s="7">
-        <v>8.5652985219278763E-2</v>
+        <f>DataRaw!J25</f>
+        <v>4.9468144799758806E-2</v>
       </c>
       <c r="AO24" s="7">
         <f t="shared" si="0"/>
@@ -4133,6 +4239,7 @@
         <v>2013</v>
       </c>
       <c r="B25" s="16">
+        <f>DataRaw!G26</f>
         <v>4.2656195131108195E-2</v>
       </c>
       <c r="C25" s="16">
@@ -4142,16 +4249,19 @@
         <v>2013</v>
       </c>
       <c r="T25" s="12">
+        <f>DataRaw!I26</f>
         <v>0.42696431913244037</v>
       </c>
       <c r="AL25" s="15">
         <v>2013</v>
       </c>
       <c r="AM25" s="16">
+        <f>DataRaw!G26</f>
         <v>4.2656195131108195E-2</v>
       </c>
       <c r="AN25" s="16">
-        <v>9.0822554345615064E-2</v>
+        <f>DataRaw!J26</f>
+        <v>5.2579371445597739E-2</v>
       </c>
       <c r="AO25" s="16">
         <f t="shared" si="0"/>
@@ -4163,6 +4273,7 @@
         <v>2014</v>
       </c>
       <c r="B26" s="16">
+        <f>DataRaw!G27</f>
         <v>4.5385307495546069E-2</v>
       </c>
       <c r="C26" s="16">
@@ -4172,16 +4283,19 @@
         <v>2014</v>
       </c>
       <c r="T26" s="12">
+        <f>DataRaw!I27</f>
         <v>0.41602855319559939</v>
       </c>
       <c r="AL26" s="15">
         <v>2014</v>
       </c>
       <c r="AM26" s="16">
+        <f>DataRaw!G27</f>
         <v>4.5385307495546069E-2</v>
       </c>
       <c r="AN26" s="16">
-        <v>9.9265533835264139E-2</v>
+        <f>DataRaw!J27</f>
+        <v>5.7692811105290613E-2</v>
       </c>
       <c r="AO26" s="16">
         <f t="shared" si="0"/>
@@ -4193,6 +4307,7 @@
         <v>2015</v>
       </c>
       <c r="B27" s="16">
+        <f>DataRaw!G28</f>
         <v>4.4417976133047585E-2</v>
       </c>
       <c r="C27" s="16">
@@ -4202,16 +4317,19 @@
         <v>2015</v>
       </c>
       <c r="T27" s="12">
+        <f>DataRaw!I28</f>
         <v>0.45636985906238581</v>
       </c>
       <c r="AL27" s="15">
         <v>2015</v>
       </c>
       <c r="AM27" s="16">
+        <f>DataRaw!G28</f>
         <v>4.4417976133047585E-2</v>
       </c>
       <c r="AN27" s="16">
-        <v>8.8456951293445982E-2</v>
+        <f>DataRaw!J28</f>
+        <v>5.1153822350645375E-2</v>
       </c>
       <c r="AO27" s="16">
         <f t="shared" si="0"/>

</xml_diff>

<commit_message>
Additional modifications to FinalProject presentation
</commit_message>
<xml_diff>
--- a/FinalProject/Docs/Townes_POLS6310_2019_Spring_FinalProject_Charts_v00.xlsx
+++ b/FinalProject/Docs/Townes_POLS6310_2019_Spring_FinalProject_Charts_v00.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405" activeTab="1"/>
+    <workbookView xWindow="390" yWindow="555" windowWidth="19815" windowHeight="9405"/>
   </bookViews>
   <sheets>
     <sheet name="DataRaw" sheetId="1" r:id="rId1"/>
@@ -320,9 +320,6 @@
     <t>Industry</t>
   </si>
   <si>
-    <t>SBIR Pct of Industry</t>
-  </si>
-  <si>
     <t>SBIR Potential</t>
   </si>
   <si>
@@ -338,7 +335,10 @@
     <t>SBIR Potential as Pct of Industry Ideal</t>
   </si>
   <si>
-    <t>Actual SBIR Pct of Industry</t>
+    <t>Actual SBIR Pct of Industry Obligations</t>
+  </si>
+  <si>
+    <t>SBIR Pct of Industry Obligations</t>
   </si>
 </sst>
 </file>
@@ -523,7 +523,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Actual SBIR Pct of Industry</c:v>
+                  <c:v>Actual SBIR Pct of Industry Obligations</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -908,11 +908,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161129216"/>
-        <c:axId val="161130752"/>
+        <c:axId val="84386560"/>
+        <c:axId val="84388096"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161129216"/>
+        <c:axId val="84386560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2015"/>
@@ -924,13 +924,13 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161130752"/>
+        <c:crossAx val="84388096"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161130752"/>
+        <c:axId val="84388096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -941,7 +941,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161129216"/>
+        <c:crossAx val="84386560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1218,11 +1218,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161146752"/>
-        <c:axId val="161148288"/>
+        <c:axId val="84404480"/>
+        <c:axId val="88154112"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161146752"/>
+        <c:axId val="84404480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2015"/>
@@ -1234,12 +1234,12 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161148288"/>
+        <c:crossAx val="88154112"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161148288"/>
+        <c:axId val="88154112"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1250,7 +1250,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161146752"/>
+        <c:crossAx val="84404480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1325,7 +1325,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Actual SBIR Pct of Industry</c:v>
+                  <c:v>Actual SBIR Pct of Industry Obligations</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1957,11 +1957,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="161304960"/>
-        <c:axId val="161306880"/>
+        <c:axId val="88171264"/>
+        <c:axId val="88173184"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="161304960"/>
+        <c:axId val="88171264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="2015"/>
@@ -1973,12 +1973,12 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161306880"/>
+        <c:crossAx val="88173184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="161306880"/>
+        <c:axId val="88173184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1989,7 +1989,7 @@
         <c:majorTickMark val="cross"/>
         <c:minorTickMark val="out"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="161304960"/>
+        <c:crossAx val="88171264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:minorUnit val="1.0000000000000002E-2"/>
@@ -2401,8 +2401,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J28"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:E1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F1" sqref="F1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2412,7 +2412,7 @@
     <col min="4" max="4" width="19.5703125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="20.140625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.28515625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="29.140625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="32.140625" bestFit="1" customWidth="1"/>
@@ -2447,16 +2447,16 @@
         <v>100</v>
       </c>
       <c r="G2" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="H2" s="13" t="s">
         <v>101</v>
       </c>
-      <c r="H2" s="13" t="s">
+      <c r="I2" s="13" t="s">
         <v>102</v>
       </c>
-      <c r="I2" s="13" t="s">
-        <v>103</v>
-      </c>
       <c r="J2" s="13" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3409,17 +3409,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AO27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AN1" workbookViewId="0">
-      <selection activeCell="BD2" sqref="BD2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AM2" sqref="AM2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6.28515625" style="6" customWidth="1"/>
-    <col min="2" max="2" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="35.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="20" max="20" width="19.140625" bestFit="1" customWidth="1"/>
     <col min="38" max="38" width="6.28515625" style="6" customWidth="1"/>
-    <col min="39" max="39" width="24.42578125" style="6" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="35.42578125" style="6" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="34.5703125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3428,28 +3428,28 @@
         <v>1</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="S1" s="14" t="s">
         <v>1</v>
       </c>
       <c r="T1" s="14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="AL1" s="5" t="s">
         <v>1</v>
       </c>
       <c r="AM1" s="5" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="AN1" s="5" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AO1" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">

</xml_diff>